<commit_message>
change calculation of F to count 'croppedarea' col if species is present on both grass and arable fields. remove balsaminaceae from adult forage plants
</commit_message>
<xml_diff>
--- a/butterfly_forage_plants.xlsx
+++ b/butterfly_forage_plants.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elinfalla/Dropbox/2020-21/_Imperial_MSc/_Project/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD60533A-5048-3E45-8993-25582BDEA4C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E724B4-1268-C345-A75F-90D7521C2894}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{D91D42CE-DEEB-2E4F-9729-BAAF2993C857}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -692,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{499D07C6-306D-9042-A539-6AA44E63D9F9}">
   <dimension ref="A1:BG49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ13" workbookViewId="0">
-      <selection activeCell="AT42" sqref="AT42"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -916,9 +916,7 @@
       <c r="G3" s="1">
         <v>1</v>
       </c>
-      <c r="H3" s="2">
-        <v>1</v>
-      </c>
+      <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="1">
@@ -1058,9 +1056,7 @@
       <c r="G5" s="1">
         <v>1</v>
       </c>
-      <c r="H5" s="2">
-        <v>1</v>
-      </c>
+      <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="1">
@@ -1207,9 +1203,7 @@
       <c r="G7" s="1">
         <v>1</v>
       </c>
-      <c r="H7" s="2">
-        <v>1</v>
-      </c>
+      <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="1">
@@ -1344,9 +1338,7 @@
       <c r="G9" s="1">
         <v>1</v>
       </c>
-      <c r="H9" s="2">
-        <v>1</v>
-      </c>
+      <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="1">
@@ -1482,9 +1474,7 @@
       <c r="G11" s="1">
         <v>1</v>
       </c>
-      <c r="H11" s="2">
-        <v>1</v>
-      </c>
+      <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="1">
@@ -1619,9 +1609,7 @@
       <c r="G13" s="1">
         <v>1</v>
       </c>
-      <c r="H13" s="2">
-        <v>1</v>
-      </c>
+      <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="1">
@@ -1756,9 +1744,7 @@
       <c r="G15" s="1">
         <v>1</v>
       </c>
-      <c r="H15" s="2">
-        <v>1</v>
-      </c>
+      <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="1">
@@ -1914,9 +1900,7 @@
       <c r="G17" s="1">
         <v>1</v>
       </c>
-      <c r="H17" s="2">
-        <v>1</v>
-      </c>
+      <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="1">
@@ -2051,9 +2035,7 @@
       <c r="G19" s="1">
         <v>1</v>
       </c>
-      <c r="H19" s="2">
-        <v>1</v>
-      </c>
+      <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="1">
@@ -2191,9 +2173,7 @@
       <c r="G21" s="1">
         <v>1</v>
       </c>
-      <c r="H21" s="2">
-        <v>1</v>
-      </c>
+      <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="1">
@@ -2328,9 +2308,7 @@
       <c r="G23" s="1">
         <v>1</v>
       </c>
-      <c r="H23" s="2">
-        <v>1</v>
-      </c>
+      <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="1">
@@ -2465,9 +2443,7 @@
       <c r="G25" s="1">
         <v>1</v>
       </c>
-      <c r="H25" s="2">
-        <v>1</v>
-      </c>
+      <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="1">
@@ -2602,9 +2578,7 @@
       <c r="G27" s="1">
         <v>1</v>
       </c>
-      <c r="H27" s="2">
-        <v>1</v>
-      </c>
+      <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="1">
@@ -2739,9 +2713,7 @@
       <c r="G29" s="1">
         <v>1</v>
       </c>
-      <c r="H29" s="2">
-        <v>1</v>
-      </c>
+      <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="1">
@@ -2879,9 +2851,7 @@
       <c r="G31" s="1">
         <v>1</v>
       </c>
-      <c r="H31" s="2">
-        <v>1</v>
-      </c>
+      <c r="H31" s="2"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="1">
@@ -3016,9 +2986,7 @@
       <c r="G33" s="1">
         <v>1</v>
       </c>
-      <c r="H33" s="2">
-        <v>1</v>
-      </c>
+      <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="1">
@@ -3153,9 +3121,7 @@
       <c r="G35" s="1">
         <v>1</v>
       </c>
-      <c r="H35" s="2">
-        <v>1</v>
-      </c>
+      <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="1">
@@ -3290,9 +3256,7 @@
       <c r="G37" s="1">
         <v>1</v>
       </c>
-      <c r="H37" s="2">
-        <v>1</v>
-      </c>
+      <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="1">
@@ -3427,9 +3391,7 @@
       <c r="G39" s="1">
         <v>1</v>
       </c>
-      <c r="H39" s="2">
-        <v>1</v>
-      </c>
+      <c r="H39" s="2"/>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="1">
@@ -3564,9 +3526,7 @@
       <c r="G41" s="1">
         <v>1</v>
       </c>
-      <c r="H41" s="2">
-        <v>1</v>
-      </c>
+      <c r="H41" s="2"/>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="1">
@@ -3704,9 +3664,7 @@
       <c r="G43" s="1">
         <v>1</v>
       </c>
-      <c r="H43" s="2">
-        <v>1</v>
-      </c>
+      <c r="H43" s="2"/>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
       <c r="K43" s="1">
@@ -3841,9 +3799,7 @@
       <c r="G45" s="1">
         <v>1</v>
       </c>
-      <c r="H45" s="2">
-        <v>1</v>
-      </c>
+      <c r="H45" s="2"/>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
       <c r="K45" s="1">
@@ -3978,9 +3934,7 @@
       <c r="G47" s="1">
         <v>1</v>
       </c>
-      <c r="H47" s="2">
-        <v>1</v>
-      </c>
+      <c r="H47" s="2"/>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
       <c r="K47" s="1">
@@ -4118,9 +4072,7 @@
       <c r="G49" s="1">
         <v>1</v>
       </c>
-      <c r="H49" s="2">
-        <v>1</v>
-      </c>
+      <c r="H49" s="2"/>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
       <c r="K49" s="1">

</xml_diff>

<commit_message>
remove resedaceae as a larval plant in butterfly plants matrix
</commit_message>
<xml_diff>
--- a/butterfly_forage_plants.xlsx
+++ b/butterfly_forage_plants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elinfalla/Dropbox/2020-21/_Imperial_MSc/_Project/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E724B4-1268-C345-A75F-90D7521C2894}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F704256C-A382-1547-9EDB-7A2223A82BE1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{D91D42CE-DEEB-2E4F-9729-BAAF2993C857}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -692,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{499D07C6-306D-9042-A539-6AA44E63D9F9}">
   <dimension ref="A1:BG49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView tabSelected="1" topLeftCell="AI9" workbookViewId="0">
+      <selection activeCell="AT21" sqref="AT21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2157,7 +2156,7 @@
         <v>1</v>
       </c>
       <c r="AT20" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:58" x14ac:dyDescent="0.2">
@@ -3648,7 +3647,7 @@
         <v>1</v>
       </c>
       <c r="AT42" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:58" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
combine bees and butterflies into butterflies script
</commit_message>
<xml_diff>
--- a/butterfly_forage_plants.xlsx
+++ b/butterfly_forage_plants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elinfalla/Dropbox/2020-21/_Imperial_MSc/_Project/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725BB1DD-CD5E-C540-84F2-7C75EDBA7AF9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801118D6-75D3-0D45-B450-95A53657371C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{D91D42CE-DEEB-2E4F-9729-BAAF2993C857}"/>
   </bookViews>
@@ -132,9 +132,6 @@
     <t>Violaceae</t>
   </si>
   <si>
-    <t>Species</t>
-  </si>
-  <si>
     <t>Brimstone</t>
   </si>
   <si>
@@ -207,9 +204,6 @@
     <t>White-letter hairstreak</t>
   </si>
   <si>
-    <t>Lifestage</t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
@@ -288,13 +282,19 @@
     <t>Valerianaceae</t>
   </si>
   <si>
-    <t>species_start</t>
-  </si>
-  <si>
-    <t>species_end</t>
-  </si>
-  <si>
     <t>Crops</t>
+  </si>
+  <si>
+    <t>plants_start</t>
+  </si>
+  <si>
+    <t>plants_end</t>
+  </si>
+  <si>
+    <t>species</t>
+  </si>
+  <si>
+    <t>lifestage</t>
   </si>
 </sst>
 </file>
@@ -698,10 +698,10 @@
   <dimension ref="A1:BH49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U43" sqref="U43"/>
+      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -718,19 +718,19 @@
   <sheetData>
     <row r="1" spans="1:60" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>84</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>0</v>
@@ -742,16 +742,16 @@
         <v>2</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>4</v>
@@ -760,7 +760,7 @@
         <v>5</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>6</v>
@@ -778,43 +778,43 @@
         <v>10</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="Y1" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Z1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="AA1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC1" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="AB1" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AC1" s="4" t="s">
-        <v>69</v>
       </c>
       <c r="AD1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="AE1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG1" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="AF1" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="AG1" s="4" t="s">
-        <v>72</v>
       </c>
       <c r="AH1" s="1" t="s">
         <v>15</v>
@@ -823,7 +823,7 @@
         <v>16</v>
       </c>
       <c r="AJ1" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AK1" s="1" t="s">
         <v>17</v>
@@ -832,7 +832,7 @@
         <v>18</v>
       </c>
       <c r="AM1" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="AN1" s="1" t="s">
         <v>19</v>
@@ -841,7 +841,7 @@
         <v>20</v>
       </c>
       <c r="AP1" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="AQ1" s="1" t="s">
         <v>21</v>
@@ -850,13 +850,13 @@
         <v>22</v>
       </c>
       <c r="AS1" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AT1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="AU1" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AV1" s="1" t="s">
         <v>24</v>
@@ -865,7 +865,7 @@
         <v>25</v>
       </c>
       <c r="AX1" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="AY1" s="1" t="s">
         <v>26</v>
@@ -874,10 +874,10 @@
         <v>27</v>
       </c>
       <c r="BA1" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="BB1" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="BC1" s="1" t="s">
         <v>28</v>
@@ -886,24 +886,24 @@
         <v>29</v>
       </c>
       <c r="BE1" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="BF1" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="BG1" s="1" t="s">
         <v>30</v>
       </c>
       <c r="BH1" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -918,10 +918,10 @@
     </row>
     <row r="3" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F3" s="1">
         <v>1</v>
@@ -1040,10 +1040,10 @@
     </row>
     <row r="4" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -1059,10 +1059,10 @@
     </row>
     <row r="5" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F5" s="1">
         <v>1</v>
@@ -1181,10 +1181,10 @@
     </row>
     <row r="6" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -1207,10 +1207,10 @@
     </row>
     <row r="7" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>
@@ -1329,10 +1329,10 @@
     </row>
     <row r="8" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -1343,10 +1343,10 @@
     </row>
     <row r="9" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F9" s="1">
         <v>1</v>
@@ -1465,10 +1465,10 @@
     </row>
     <row r="10" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -1480,10 +1480,10 @@
     </row>
     <row r="11" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F11" s="1">
         <v>1</v>
@@ -1602,10 +1602,10 @@
     </row>
     <row r="12" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -1616,10 +1616,10 @@
     </row>
     <row r="13" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F13" s="1">
         <v>1</v>
@@ -1738,10 +1738,10 @@
     </row>
     <row r="14" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L14">
         <v>0</v>
@@ -1752,10 +1752,10 @@
     </row>
     <row r="15" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F15" s="1">
         <v>1</v>
@@ -1874,10 +1874,10 @@
     </row>
     <row r="16" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -1909,10 +1909,10 @@
     </row>
     <row r="17" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F17" s="1">
         <v>1</v>
@@ -2031,10 +2031,10 @@
     </row>
     <row r="18" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L18">
         <v>0</v>
@@ -2045,10 +2045,10 @@
     </row>
     <row r="19" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F19" s="1">
         <v>1</v>
@@ -2167,10 +2167,10 @@
     </row>
     <row r="20" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L20">
         <v>0</v>
@@ -2187,10 +2187,10 @@
     </row>
     <row r="21" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F21" s="1">
         <v>1</v>
@@ -2309,10 +2309,10 @@
     </row>
     <row r="22" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L22">
         <v>0</v>
@@ -2323,10 +2323,10 @@
     </row>
     <row r="23" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F23" s="1">
         <v>1</v>
@@ -2445,10 +2445,10 @@
     </row>
     <row r="24" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L24">
         <v>0</v>
@@ -2459,10 +2459,10 @@
     </row>
     <row r="25" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F25" s="1">
         <v>1</v>
@@ -2581,10 +2581,10 @@
     </row>
     <row r="26" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B26" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L26">
         <v>0</v>
@@ -2595,10 +2595,10 @@
     </row>
     <row r="27" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F27" s="1">
         <v>1</v>
@@ -2717,10 +2717,10 @@
     </row>
     <row r="28" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B28" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L28">
         <v>0</v>
@@ -2731,10 +2731,10 @@
     </row>
     <row r="29" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F29" s="1">
         <v>1</v>
@@ -2853,10 +2853,10 @@
     </row>
     <row r="30" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L30">
         <v>0</v>
@@ -2870,10 +2870,10 @@
     </row>
     <row r="31" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B31" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F31" s="1">
         <v>1</v>
@@ -2992,10 +2992,10 @@
     </row>
     <row r="32" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B32" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L32">
         <v>0</v>
@@ -3006,10 +3006,10 @@
     </row>
     <row r="33" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F33" s="1">
         <v>1</v>
@@ -3128,10 +3128,10 @@
     </row>
     <row r="34" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B34" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L34">
         <v>0</v>
@@ -3142,10 +3142,10 @@
     </row>
     <row r="35" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B35" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F35" s="1">
         <v>1</v>
@@ -3264,10 +3264,10 @@
     </row>
     <row r="36" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B36" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L36">
         <v>0</v>
@@ -3278,10 +3278,10 @@
     </row>
     <row r="37" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B37" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F37" s="1">
         <v>1</v>
@@ -3400,10 +3400,10 @@
     </row>
     <row r="38" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B38" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L38">
         <v>0</v>
@@ -3414,10 +3414,10 @@
     </row>
     <row r="39" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B39" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F39" s="1">
         <v>1</v>
@@ -3536,10 +3536,10 @@
     </row>
     <row r="40" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B40" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L40">
         <v>0</v>
@@ -3550,10 +3550,10 @@
     </row>
     <row r="41" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B41" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F41" s="1">
         <v>1</v>
@@ -3672,10 +3672,10 @@
     </row>
     <row r="42" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B42" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L42">
         <v>0</v>
@@ -3692,10 +3692,10 @@
     </row>
     <row r="43" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B43" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F43" s="1">
         <v>1</v>
@@ -3814,10 +3814,10 @@
     </row>
     <row r="44" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B44" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L44">
         <v>0</v>
@@ -3828,10 +3828,10 @@
     </row>
     <row r="45" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B45" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F45" s="1">
         <v>1</v>
@@ -3950,10 +3950,10 @@
     </row>
     <row r="46" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B46" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L46">
         <v>0</v>
@@ -3964,10 +3964,10 @@
     </row>
     <row r="47" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B47" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F47" s="1">
         <v>1</v>
@@ -4086,10 +4086,10 @@
     </row>
     <row r="48" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C48" s="6"/>
       <c r="D48" s="3"/>
@@ -4103,10 +4103,10 @@
     </row>
     <row r="49" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B49" t="s">
         <v>55</v>
-      </c>
-      <c r="B49" t="s">
-        <v>57</v>
       </c>
       <c r="F49" s="1">
         <v>1</v>

</xml_diff>